<commit_message>
Budget US sheet Updated
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Budget_Anonymous_CA.xlsx
+++ b/budget-web-tests/testData/Budget_Anonymous_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/Budget_Payless 27 Apr/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A20BA78-A5AC-114C-AB1D-9BFB13FA2FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D05AB8-BC5F-A649-965D-E74291DFB7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="121">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -245,18 +245,6 @@
     <t>Thailand</t>
   </si>
   <si>
-    <t>UUZZ011</t>
-  </si>
-  <si>
-    <t>04/13/2023</t>
-  </si>
-  <si>
-    <t>04/18/2023</t>
-  </si>
-  <si>
-    <t>TUZZ008</t>
-  </si>
-  <si>
     <t>Delta</t>
   </si>
   <si>
@@ -266,9 +254,6 @@
     <t>YYZ</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Budget_RES_Modify_cancel_flow_Step1_to_Step4_CA</t>
   </si>
   <si>
@@ -393,6 +378,12 @@
   </si>
   <si>
     <t>Paynow</t>
+  </si>
+  <si>
+    <t>Verify</t>
+  </si>
+  <si>
+    <t>LHR</t>
   </si>
 </sst>
 </file>
@@ -401,9 +392,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +456,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -488,7 +491,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -500,9 +503,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -528,6 +528,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -808,7 +817,7 @@
   <dimension ref="A1:BR22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,58 +994,58 @@
       <c r="BC1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="BH1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="BI1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BJ1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BK1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BL1" t="s">
         <v>112</v>
       </c>
-      <c r="BH1" s="10" t="s">
+      <c r="BM1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="BI1" s="10" t="s">
+      <c r="BN1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="BJ1" s="10" t="s">
+      <c r="BO1" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BP1" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BQ1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="BM1" s="11" t="s">
+      <c r="BR1" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="BN1" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BP1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="BQ1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="BR1" s="12" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>108</v>
+      <c r="A2" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>55</v>
@@ -1048,10 +1057,10 @@
         <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>56</v>
@@ -1197,37 +1206,37 @@
       <c r="BC2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN2" s="13" t="s">
+      <c r="BD2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN2" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO2" t="s">
@@ -1244,11 +1253,11 @@
       </c>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>108</v>
+      <c r="A3" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>55</v>
@@ -1260,10 +1269,10 @@
         <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
         <v>62</v>
@@ -1332,10 +1341,10 @@
         <v>66</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>56</v>
@@ -1409,37 +1418,37 @@
       <c r="BC3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BD3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN3" s="13" t="s">
+      <c r="BD3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN3" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO3" t="s">
@@ -1456,11 +1465,11 @@
       </c>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>108</v>
+      <c r="A4" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>55</v>
@@ -1472,10 +1481,10 @@
         <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
         <v>62</v>
@@ -1621,37 +1630,37 @@
       <c r="BC4" t="s">
         <v>56</v>
       </c>
-      <c r="BD4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN4" s="13" t="s">
+      <c r="BD4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN4" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO4" t="s">
@@ -1668,11 +1677,11 @@
       </c>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>108</v>
+      <c r="A5" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -1686,8 +1695,8 @@
       <c r="F5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G5" t="s">
-        <v>81</v>
+      <c r="G5" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>62</v>
@@ -1761,10 +1770,10 @@
       <c r="AE5" t="s">
         <v>56</v>
       </c>
-      <c r="AF5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AF5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG5" s="8" t="s">
         <v>56</v>
       </c>
       <c r="AH5" t="s">
@@ -1833,37 +1842,37 @@
       <c r="BC5" t="s">
         <v>56</v>
       </c>
-      <c r="BD5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL5" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM5" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN5" s="13" t="s">
+      <c r="BD5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN5" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO5" t="s">
@@ -1880,11 +1889,11 @@
       </c>
     </row>
     <row r="6" spans="1:70" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>108</v>
+      <c r="A6" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>55</v>
@@ -1896,18 +1905,18 @@
         <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>56</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>56</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1997,7 +2006,7 @@
       <c r="AM6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AN6" s="8" t="s">
+      <c r="AN6" s="7" t="s">
         <v>56</v>
       </c>
       <c r="AO6" s="2" t="s">
@@ -2039,43 +2048,43 @@
       <c r="BA6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BB6" s="7" t="s">
-        <v>78</v>
+      <c r="BB6" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="BC6">
         <v>2323</v>
       </c>
-      <c r="BD6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN6" s="13" t="s">
+      <c r="BD6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN6" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO6" t="s">
@@ -2092,11 +2101,11 @@
       </c>
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>108</v>
+      <c r="A7" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
@@ -2108,10 +2117,10 @@
         <v>56</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
         <v>62</v>
@@ -2180,15 +2189,15 @@
         <v>66</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF7" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AG7" s="15">
         <v>38298026</v>
       </c>
       <c r="AH7" s="2" t="s">
@@ -2252,42 +2261,42 @@
         <v>56</v>
       </c>
       <c r="BB7" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC7" s="2">
         <v>2323</v>
       </c>
-      <c r="BD7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN7" s="13" t="s">
+      <c r="BD7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN7" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO7" t="s">
@@ -2304,11 +2313,11 @@
       </c>
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>108</v>
+      <c r="A8" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>55</v>
@@ -2320,10 +2329,10 @@
         <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
         <v>62</v>
@@ -2338,7 +2347,7 @@
         <v>56</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>56</v>
@@ -2464,42 +2473,42 @@
         <v>56</v>
       </c>
       <c r="BB8" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC8" s="2">
         <v>2323</v>
       </c>
-      <c r="BD8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG8" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN8" s="13" t="s">
+      <c r="BD8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN8" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO8" t="s">
@@ -2516,11 +2525,11 @@
       </c>
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>108</v>
+      <c r="A9" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>55</v>
@@ -2532,10 +2541,10 @@
         <v>56</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>56</v>
@@ -2676,42 +2685,42 @@
         <v>56</v>
       </c>
       <c r="BB9" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC9" s="2">
         <v>2323</v>
       </c>
-      <c r="BD9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN9" s="13" t="s">
+      <c r="BD9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN9" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO9" t="s">
@@ -2728,11 +2737,11 @@
       </c>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>108</v>
+      <c r="A10" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>55</v>
@@ -2744,7 +2753,7 @@
         <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
         <v>73</v>
@@ -2888,42 +2897,42 @@
         <v>56</v>
       </c>
       <c r="BB10" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC10" s="2">
         <v>2323</v>
       </c>
-      <c r="BD10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN10" s="13" t="s">
+      <c r="BD10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN10" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO10" t="s">
@@ -2940,11 +2949,11 @@
       </c>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>108</v>
+      <c r="A11" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
         <v>55</v>
@@ -2956,18 +2965,18 @@
         <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="K11" t="s">
@@ -3033,7 +3042,7 @@
       <c r="AE11" t="s">
         <v>56</v>
       </c>
-      <c r="AF11" s="8" t="s">
+      <c r="AF11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="AG11" t="s">
@@ -3057,7 +3066,7 @@
       <c r="AM11" t="s">
         <v>56</v>
       </c>
-      <c r="AN11" s="8" t="s">
+      <c r="AN11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="AO11" t="s">
@@ -3100,42 +3109,42 @@
         <v>56</v>
       </c>
       <c r="BB11" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC11" s="2">
         <v>2323</v>
       </c>
-      <c r="BD11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN11" s="13" t="s">
+      <c r="BD11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO11" t="s">
@@ -3152,11 +3161,11 @@
       </c>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>108</v>
+      <c r="A12" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>55</v>
@@ -3168,19 +3177,19 @@
         <v>56</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
         <v>56</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
         <v>56</v>
@@ -3188,8 +3197,8 @@
       <c r="L12" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="8" t="s">
-        <v>74</v>
+      <c r="M12" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="N12" t="s">
         <v>56</v>
@@ -3312,42 +3321,42 @@
         <v>56</v>
       </c>
       <c r="BB12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC12">
         <v>2323</v>
       </c>
-      <c r="BD12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN12" s="13" t="s">
+      <c r="BD12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN12" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO12" t="s">
@@ -3364,11 +3373,11 @@
       </c>
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>108</v>
+      <c r="A13" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -3380,7 +3389,7 @@
         <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
         <v>56</v>
@@ -3457,10 +3466,10 @@
       <c r="AE13" t="s">
         <v>56</v>
       </c>
-      <c r="AF13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG13" s="9" t="s">
+      <c r="AF13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG13" s="8" t="s">
         <v>56</v>
       </c>
       <c r="AH13" t="s">
@@ -3524,42 +3533,42 @@
         <v>56</v>
       </c>
       <c r="BB13" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC13" s="2">
         <v>2323</v>
       </c>
-      <c r="BD13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL13" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM13" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN13" s="13" t="s">
+      <c r="BD13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN13" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO13" t="s">
@@ -3576,11 +3585,11 @@
       </c>
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>108</v>
+      <c r="A14" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>55</v>
@@ -3592,7 +3601,7 @@
         <v>56</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s">
         <v>56</v>
@@ -3736,42 +3745,42 @@
         <v>56</v>
       </c>
       <c r="BB14" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC14" s="2">
         <v>2323</v>
       </c>
-      <c r="BD14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN14" s="13" t="s">
+      <c r="BD14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN14" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO14" t="s">
@@ -3788,14 +3797,14 @@
       </c>
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>108</v>
+      <c r="A15" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
+        <v>94</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
@@ -3804,19 +3813,19 @@
         <v>56</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
         <v>56</v>
       </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" t="s">
-        <v>63</v>
+      <c r="H15" s="16">
+        <v>45118</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="16">
+        <v>45210</v>
       </c>
       <c r="K15" t="s">
         <v>56</v>
@@ -3839,20 +3848,20 @@
       <c r="Q15" t="s">
         <v>56</v>
       </c>
-      <c r="R15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T15" t="s">
-        <v>60</v>
-      </c>
-      <c r="U15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V15" s="3">
-        <v>9838234567</v>
+      <c r="R15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="V15" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="W15" t="s">
         <v>56</v>
@@ -3947,43 +3956,43 @@
       <c r="BA15" t="s">
         <v>56</v>
       </c>
-      <c r="BB15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BC15" s="2">
-        <v>2323</v>
-      </c>
-      <c r="BD15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN15" s="13" t="s">
+      <c r="BB15" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BL15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BN15" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO15" t="s">
@@ -4000,11 +4009,11 @@
       </c>
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>108</v>
+      <c r="A16" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
@@ -4016,19 +4025,19 @@
         <v>56</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G16" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>75</v>
+      <c r="H16" t="s">
+        <v>62</v>
       </c>
       <c r="I16" t="s">
         <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
         <v>56</v>
@@ -4036,12 +4045,10 @@
       <c r="L16" t="s">
         <v>56</v>
       </c>
-      <c r="M16" t="s">
-        <v>56</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="M16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" s="7"/>
       <c r="O16" t="s">
         <v>56</v>
       </c>
@@ -4160,42 +4167,42 @@
         <v>56</v>
       </c>
       <c r="BB16" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC16" s="2">
         <v>2323</v>
       </c>
-      <c r="BD16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN16" s="13" t="s">
+      <c r="BD16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO16" t="s">
@@ -4212,11 +4219,11 @@
       </c>
     </row>
     <row r="17" spans="1:70" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>108</v>
+      <c r="A17" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
@@ -4228,7 +4235,7 @@
         <v>56</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
         <v>56</v>
@@ -4371,43 +4378,43 @@
       <c r="BA17" t="s">
         <v>56</v>
       </c>
-      <c r="BB17" s="7" t="s">
-        <v>78</v>
+      <c r="BB17" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="BC17">
         <v>2323</v>
       </c>
-      <c r="BD17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN17" s="13" t="s">
+      <c r="BD17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL17" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM17" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN17" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BO17" t="s">
@@ -4424,11 +4431,11 @@
       </c>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>108</v>
+      <c r="A18" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
         <v>55</v>
@@ -4440,7 +4447,7 @@
         <v>56</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G18" t="s">
         <v>56</v>
@@ -4584,45 +4591,45 @@
         <v>56</v>
       </c>
       <c r="BB18" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC18" s="2">
         <v>2323</v>
       </c>
-      <c r="BD18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO18" s="8" t="s">
+      <c r="BD18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO18" s="7" t="s">
         <v>56</v>
       </c>
       <c r="BP18" t="s">
@@ -4636,11 +4643,11 @@
       </c>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>108</v>
+      <c r="A19" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
         <v>55</v>
@@ -4652,19 +4659,19 @@
         <v>56</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
       </c>
       <c r="I19" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>56</v>
+      <c r="J19" t="s">
+        <v>63</v>
       </c>
       <c r="K19" t="s">
         <v>56</v>
@@ -4672,8 +4679,8 @@
       <c r="L19" t="s">
         <v>56</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>74</v>
+      <c r="M19" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="N19" t="s">
         <v>56</v>
@@ -4796,51 +4803,51 @@
         <v>56</v>
       </c>
       <c r="BB19" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC19" s="2">
         <v>2323</v>
       </c>
-      <c r="BD19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BP19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BQ19" s="14" t="s">
+      <c r="BD19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BP19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BQ19" s="13" t="s">
         <v>56</v>
       </c>
       <c r="BR19" t="s">
@@ -4848,11 +4855,11 @@
       </c>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>108</v>
+      <c r="A20" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -4864,7 +4871,7 @@
         <v>56</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
         <v>56</v>
@@ -4936,10 +4943,10 @@
         <v>66</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AF20" t="s">
         <v>56</v>
@@ -4956,7 +4963,7 @@
       <c r="AJ20" t="s">
         <v>56</v>
       </c>
-      <c r="AK20" s="8" t="s">
+      <c r="AK20" s="7" t="s">
         <v>56</v>
       </c>
       <c r="AL20" t="s">
@@ -5008,45 +5015,45 @@
         <v>56</v>
       </c>
       <c r="BB20" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC20" s="2">
         <v>2323</v>
       </c>
-      <c r="BD20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO20" s="13" t="s">
+      <c r="BD20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO20" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BP20" t="s">
@@ -5060,11 +5067,11 @@
       </c>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>108</v>
+      <c r="A21" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
         <v>55</v>
@@ -5076,7 +5083,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
         <v>56</v>
@@ -5148,10 +5155,10 @@
         <v>66</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AF21" t="s">
         <v>56</v>
@@ -5168,7 +5175,7 @@
       <c r="AJ21" t="s">
         <v>56</v>
       </c>
-      <c r="AK21" s="8" t="s">
+      <c r="AK21" s="7" t="s">
         <v>56</v>
       </c>
       <c r="AL21" t="s">
@@ -5220,45 +5227,45 @@
         <v>56</v>
       </c>
       <c r="BB21" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="BC21" s="2">
         <v>2323</v>
       </c>
-      <c r="BD21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE21" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF21" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG21" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BK21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BM21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO21" s="13" t="s">
+      <c r="BD21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BL21" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BM21" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN21" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO21" s="12" t="s">
         <v>56</v>
       </c>
       <c r="BP21" t="s">
@@ -5300,10 +5307,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -5452,7 +5459,7 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>55</v>

</xml_diff>